<commit_message>
Update files and schemas
</commit_message>
<xml_diff>
--- a/optoelectronics/solar_cell_custom_ELN/jv_file.xlsx
+++ b/optoelectronics/solar_cell_custom_ELN/jv_file.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\pepe_marquez\AreaE\AreaE_use-cases\optoelectronics\solar_cell_custom_ELN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5AA660B-FB53-401B-9ED4-3BF694EB75BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38B8852B-3040-4DFD-B74A-1B2E9BC7E3BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{9B62EA0A-E572-4D87-8737-89E1F46C4964}"/>
+    <workbookView xWindow="-38510" yWindow="-5520" windowWidth="38620" windowHeight="21100" xr2:uid="{9B62EA0A-E572-4D87-8737-89E1F46C4964}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -393,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4304455F-D541-4F31-9DD5-E57B587BCC33}">
-  <dimension ref="A1:G74"/>
+  <dimension ref="A1:F161"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -404,7 +404,7 @@
     <col min="1" max="2" width="15.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -412,954 +412,1577 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
-        <v>1.25</v>
+        <v>-0.59718293887997898</v>
       </c>
       <c r="B2" s="1">
-        <v>10.258900000000001</v>
+        <v>-32.791159821751101</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
-        <v>1.23</v>
+        <v>-0.58645575156728302</v>
       </c>
       <c r="B3" s="1">
-        <v>4.4411769999999997</v>
+        <v>-32.791159821751101</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
-        <v>1.21</v>
+        <v>-0.57572856425458796</v>
       </c>
       <c r="B4" s="1">
-        <v>-0.71184250000000004</v>
+        <v>-32.791159821751101</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
-        <v>1.19</v>
+        <v>-0.56500137694189301</v>
       </c>
       <c r="B5" s="1">
-        <v>-5.2578440000000004</v>
+        <v>-32.791159821751101</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
-        <v>1.17</v>
+        <v>-0.55427418962919695</v>
       </c>
       <c r="B6" s="1">
-        <v>-9.1271559999999994</v>
+        <v>-32.791159821751101</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
-        <v>1.1499999999999999</v>
+        <v>-0.54354700231650199</v>
       </c>
       <c r="B7" s="1">
-        <v>-12.420360000000001</v>
+        <v>-32.791159821751101</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
-        <v>1.1299999999999999</v>
+        <v>-0.53281981500380604</v>
       </c>
       <c r="B8" s="1">
-        <v>-15.055149999999999</v>
+        <v>-32.791159821751101</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
-        <v>1.1100000000000001</v>
+        <v>-0.52209262769111098</v>
       </c>
       <c r="B9" s="1">
-        <v>-17.060780000000001</v>
+        <v>-32.791159821751101</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
-        <v>1.0900000000000001</v>
+        <v>-0.51136544037841603</v>
       </c>
       <c r="B10" s="1">
-        <v>-18.520479999999999</v>
+        <v>-32.791159821751101</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
-        <v>1.07</v>
+        <v>-0.50063825306571996</v>
       </c>
       <c r="B11" s="1">
-        <v>-19.549959999999999</v>
+        <v>-32.791159821751101</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
-        <v>1.05</v>
+        <v>-0.48991106575302501</v>
       </c>
       <c r="B12" s="1">
-        <v>-20.24381</v>
+        <v>-32.791159821751101</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
-        <v>1.03</v>
+        <v>-0.479183878440329</v>
       </c>
       <c r="B13" s="1">
-        <v>-20.70064</v>
+        <v>-32.703276289329501</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
-        <v>1.01</v>
+        <v>-0.468456691127634</v>
       </c>
       <c r="B14" s="1">
-        <v>-20.989570000000001</v>
+        <v>-32.6703199646713</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
-        <v>0.99</v>
+        <v>-0.45772950381493899</v>
       </c>
       <c r="B15" s="1">
-        <v>-21.179950000000002</v>
+        <v>-32.6703199646713</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
-        <v>0.97</v>
+        <v>-0.44700231650224298</v>
       </c>
       <c r="B16" s="1">
-        <v>-21.308689999999999</v>
+        <v>-32.6703199646713</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
-        <v>0.95</v>
+        <v>-0.43627512918954803</v>
       </c>
       <c r="B17" s="1">
-        <v>-21.413460000000001</v>
+        <v>-32.6703199646713</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
-        <v>0.93</v>
+        <v>-0.42554794187685202</v>
       </c>
       <c r="B18" s="1">
-        <v>-21.47437</v>
+        <v>-32.6703199646713</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
-        <v>0.91</v>
+        <v>-0.41482075456415701</v>
       </c>
       <c r="B19" s="1">
-        <v>-21.534210000000002</v>
+        <v>-32.6703199646713</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
-        <v>0.89</v>
+        <v>-0.404093567251462</v>
       </c>
       <c r="B20" s="1">
-        <v>-21.56888</v>
+        <v>-32.6703199646713</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
-        <v>0.87</v>
+        <v>-0.393366379938766</v>
       </c>
       <c r="B21" s="1">
-        <v>-21.612220000000001</v>
+        <v>-32.6703199646713</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
-        <v>0.85</v>
+        <v>-0.38263919262607099</v>
       </c>
       <c r="B22" s="1">
-        <v>-21.64969</v>
+        <v>-32.6703199646713</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
-        <v>0.83</v>
+        <v>-0.37191200531337498</v>
       </c>
       <c r="B23" s="1">
-        <v>-21.67409</v>
+        <v>-32.6703199646713</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
-        <v>0.81</v>
+        <v>-0.36118481800067997</v>
       </c>
       <c r="B24" s="1">
-        <v>-21.705539999999999</v>
+        <v>-32.6703199646713</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
-        <v>0.79</v>
+        <v>-0.35045763068798402</v>
       </c>
       <c r="B25" s="1">
-        <v>-21.71649</v>
+        <v>-32.6703199646713</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
-        <v>0.77</v>
+        <v>-0.33973044337528902</v>
       </c>
       <c r="B26" s="1">
-        <v>-21.743639999999999</v>
+        <v>-32.6703199646713</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
-        <v>0.75</v>
+        <v>-0.32900325606259401</v>
       </c>
       <c r="B27" s="1">
-        <v>-21.76859</v>
+        <v>-32.6703199646713</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
-        <v>0.73</v>
+        <v>-0.318276068749898</v>
       </c>
       <c r="B28" s="1">
-        <v>-21.76398</v>
+        <v>-32.571450990697002</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
-        <v>0.71</v>
+        <v>-0.30754888143720299</v>
       </c>
       <c r="B29" s="1">
-        <v>-21.77779</v>
+        <v>-32.549480107591599</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
-        <v>0.69</v>
+        <v>-0.29682169412450798</v>
       </c>
       <c r="B30" s="1">
-        <v>-21.791429999999998</v>
+        <v>-32.549480107591599</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
-        <v>0.67</v>
+        <v>-0.28609450681181198</v>
       </c>
       <c r="B31" s="1">
-        <v>-21.805890000000002</v>
+        <v>-32.549480107591599</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
-        <v>0.65</v>
+        <v>-0.27536731949911702</v>
       </c>
       <c r="B32" s="1">
-        <v>-21.834330000000001</v>
+        <v>-32.549480107591599</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
-        <v>0.63</v>
+        <v>-0.26464013218642102</v>
       </c>
       <c r="B33" s="1">
-        <v>-21.837409999999998</v>
+        <v>-32.538494666038901</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
-        <v>0.61</v>
+        <v>-0.25391294487372601</v>
       </c>
       <c r="B34" s="1">
-        <v>-21.84731</v>
+        <v>-32.428640250511798</v>
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
-        <v>0.59</v>
+        <v>-0.243185757561031</v>
       </c>
       <c r="B35" s="1">
-        <v>-21.847270000000002</v>
+        <v>-32.428640250511798</v>
       </c>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
-        <v>0.56999999999999995</v>
+        <v>-0.23245857024833499</v>
       </c>
       <c r="B36" s="1">
-        <v>-21.86279</v>
+        <v>-32.428640250511798</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
-        <v>0.55000000000000004</v>
+        <v>-0.22173138293563999</v>
       </c>
       <c r="B37" s="1">
-        <v>-21.870090000000001</v>
+        <v>-32.428640250511798</v>
       </c>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
-        <v>0.53</v>
+        <v>-0.21100419562294401</v>
       </c>
       <c r="B38" s="1">
-        <v>-21.873660000000001</v>
+        <v>-32.428640250511798</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
-        <v>0.51</v>
+        <v>-0.200277008310249</v>
       </c>
       <c r="B39" s="1">
-        <v>-21.869119999999999</v>
+        <v>-32.428640250511798</v>
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
-        <v>0.49</v>
+        <v>-0.18954982099755299</v>
       </c>
       <c r="B40" s="1">
-        <v>-21.883800000000001</v>
+        <v>-32.428640250511798</v>
       </c>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
-        <v>0.47</v>
+        <v>-0.17882263368485801</v>
       </c>
       <c r="B41" s="1">
-        <v>-21.89226</v>
+        <v>-32.428640250511798</v>
       </c>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
-        <v>0.45</v>
+        <v>-0.168095446372163</v>
       </c>
       <c r="B42" s="1">
-        <v>-21.908000000000001</v>
+        <v>-32.428640250511798</v>
       </c>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
-        <v>0.43</v>
+        <v>-0.157368259059467</v>
       </c>
       <c r="B43" s="1">
-        <v>-21.908049999999999</v>
+        <v>-32.3297712765375</v>
       </c>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
-        <v>0.41</v>
+        <v>-0.14664107174677199</v>
       </c>
       <c r="B44" s="1">
-        <v>-21.906870000000001</v>
+        <v>-32.307800393432103</v>
       </c>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
-        <v>0.39</v>
+        <v>-0.13591388443407601</v>
       </c>
       <c r="B45" s="1">
-        <v>-21.919329999999999</v>
+        <v>-32.307800393432103</v>
       </c>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
-      <c r="G45" s="1"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
-        <v>0.37</v>
+        <v>-0.125186697121381</v>
       </c>
       <c r="B46" s="1">
-        <v>-21.914580000000001</v>
+        <v>-32.307800393432103</v>
       </c>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
-      <c r="G46" s="1"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
-        <v>0.35</v>
+        <v>-0.11445950980868599</v>
       </c>
       <c r="B47" s="1">
-        <v>-21.930240000000001</v>
+        <v>-32.307800393432103</v>
       </c>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
-      <c r="G47" s="1"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
-        <v>0.33</v>
+        <v>-0.10373232249599</v>
       </c>
       <c r="B48" s="1">
-        <v>-21.921389999999999</v>
+        <v>-32.274844068773902</v>
       </c>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
-      <c r="G48" s="1"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
-        <v>0.31</v>
+        <v>-9.3005135183295298E-2</v>
       </c>
       <c r="B49" s="1">
-        <v>-21.93365</v>
+        <v>-32.186960536352302</v>
       </c>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
-      <c r="G49" s="1"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
-        <v>0.28999999999999998</v>
+        <v>-8.2277947870599902E-2</v>
       </c>
       <c r="B50" s="1">
-        <v>-21.93319</v>
+        <v>-32.186960536352302</v>
       </c>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
-      <c r="G50" s="1"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
-        <v>0.27</v>
+        <v>-7.1550760557904505E-2</v>
       </c>
       <c r="B51" s="1">
-        <v>-21.946840000000002</v>
+        <v>-32.186960536352302</v>
       </c>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
-      <c r="G51" s="1"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52" s="1">
-        <v>0.25</v>
+        <v>-6.0823573245209102E-2</v>
       </c>
       <c r="B52" s="1">
-        <v>-21.951219999999999</v>
+        <v>-32.186960536352302</v>
       </c>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
-      <c r="G52" s="1"/>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" s="1">
-        <v>0.23</v>
+        <v>-5.0096385932513698E-2</v>
       </c>
       <c r="B53" s="1">
-        <v>-21.95383</v>
+        <v>-32.186960536352302</v>
       </c>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
-      <c r="G53" s="1"/>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
-        <v>0.21</v>
+        <v>-3.9369198619818302E-2</v>
       </c>
       <c r="B54" s="1">
-        <v>-21.960619999999999</v>
+        <v>-32.121047887036099</v>
       </c>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
-      <c r="G54" s="1"/>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
-        <v>0.19</v>
+        <v>-2.8642011307122899E-2</v>
       </c>
       <c r="B55" s="1">
-        <v>-21.96546</v>
+        <v>-32.066120679272501</v>
       </c>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
-      <c r="G55" s="1"/>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" s="1">
-        <v>0.17</v>
+        <v>-1.7914823994427499E-2</v>
       </c>
       <c r="B56" s="1">
-        <v>-21.97579</v>
+        <v>-32.066120679272501</v>
       </c>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
-      <c r="G56" s="1"/>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57" s="1">
-        <v>0.15</v>
+        <v>-7.1876366817321602E-3</v>
       </c>
       <c r="B57" s="1">
-        <v>-21.973960000000002</v>
+        <v>-32.066120679272501</v>
       </c>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
-      <c r="G57" s="1"/>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58" s="1">
-        <v>0.13</v>
+        <v>7.4403460173979499E-3</v>
       </c>
       <c r="B58" s="1">
-        <v>-21.969860000000001</v>
+        <v>-32.066120679272501</v>
       </c>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
-      <c r="G58" s="1"/>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
-        <v>0.11</v>
+        <v>1.81675333300933E-2</v>
       </c>
       <c r="B59" s="1">
-        <v>-21.97719</v>
+        <v>-32.022178913061701</v>
       </c>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
-      <c r="G59" s="1"/>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60" s="1">
-        <v>0.09</v>
+        <v>2.8894720642788699E-2</v>
       </c>
       <c r="B60" s="1">
-        <v>-21.983709999999999</v>
+        <v>-31.9452808221927</v>
       </c>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
-      <c r="G60" s="1"/>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61" s="1">
-        <v>7.0000000000000007E-2</v>
+        <v>3.9621907955484099E-2</v>
       </c>
       <c r="B61" s="1">
-        <v>-21.98509</v>
+        <v>-31.9452808221927</v>
       </c>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>
-      <c r="G61" s="1"/>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62" s="1">
-        <v>0.05</v>
+        <v>5.0349095268179503E-2</v>
       </c>
       <c r="B62" s="1">
-        <v>-21.98931</v>
+        <v>-31.9452808221927</v>
       </c>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
-      <c r="G62" s="1"/>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
-        <v>0.03</v>
+        <v>6.1076282580874899E-2</v>
       </c>
       <c r="B63" s="1">
-        <v>-21.984760000000001</v>
+        <v>-31.868382731323798</v>
       </c>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
-      <c r="G63" s="1"/>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64" s="1">
-        <v>0.01</v>
+        <v>7.1803469893570296E-2</v>
       </c>
       <c r="B64" s="1">
-        <v>-21.989599999999999</v>
+        <v>-31.824440965112998</v>
       </c>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
       <c r="F64" s="1"/>
-      <c r="G64" s="1"/>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
-        <v>-0.01</v>
+        <v>8.2530657206265803E-2</v>
       </c>
       <c r="B65" s="1">
-        <v>-21.991340000000001</v>
+        <v>-31.785991919678501</v>
       </c>
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
       <c r="E65" s="1"/>
       <c r="F65" s="1"/>
-      <c r="G65" s="1"/>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66" s="1">
-        <v>-0.03</v>
+        <v>9.3257844518961103E-2</v>
       </c>
       <c r="B66" s="1">
-        <v>-21.995719999999999</v>
+        <v>-31.764021036573101</v>
       </c>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
       <c r="F66" s="1"/>
-      <c r="G66" s="1"/>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67" s="1">
-        <v>-0.05</v>
+        <v>0.103985031831656</v>
       </c>
       <c r="B67" s="1">
-        <v>-22.00338</v>
+        <v>-31.7090938288095</v>
       </c>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
       <c r="F67" s="1"/>
-      <c r="G67" s="1"/>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68" s="1">
-        <v>-7.0000000000000007E-2</v>
+        <v>0.11471221914435099</v>
       </c>
       <c r="B68" s="1">
-        <v>-21.999700000000001</v>
+        <v>-31.703601108033201</v>
       </c>
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
-      <c r="G68" s="1"/>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69" s="1">
-        <v>-0.09</v>
+        <v>0.12543940645704699</v>
       </c>
       <c r="B69" s="1">
-        <v>-22.008209999999998</v>
+        <v>-31.5827612509534</v>
       </c>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
       <c r="E69" s="1"/>
       <c r="F69" s="1"/>
-      <c r="G69" s="1"/>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70" s="1">
-        <v>-0.11</v>
+        <v>0.13616659376974199</v>
       </c>
       <c r="B70" s="1">
-        <v>-22.01539</v>
+        <v>-31.5827612509534</v>
       </c>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
       <c r="E70" s="1"/>
       <c r="F70" s="1"/>
-      <c r="G70" s="1"/>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71" s="1">
-        <v>-0.13</v>
+        <v>0.146893781082438</v>
       </c>
       <c r="B71" s="1">
-        <v>-22.01962</v>
+        <v>-31.5827612509534</v>
       </c>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
       <c r="E71" s="1"/>
       <c r="F71" s="1"/>
-      <c r="G71" s="1"/>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72" s="1">
-        <v>-0.15</v>
+        <v>0.15762096839513301</v>
       </c>
       <c r="B72" s="1">
-        <v>-22.026879999999998</v>
+        <v>-31.4948777185318</v>
       </c>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
       <c r="E72" s="1"/>
       <c r="F72" s="1"/>
-      <c r="G72" s="1"/>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73" s="1">
-        <v>-0.17</v>
+        <v>0.16834815570782899</v>
       </c>
       <c r="B73" s="1">
-        <v>-22.025269999999999</v>
+        <v>-31.461921393873599</v>
       </c>
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
       <c r="E73" s="1"/>
       <c r="F73" s="1"/>
-      <c r="G73" s="1"/>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74" s="1">
-        <v>-0.19</v>
+        <v>0.179075343020524</v>
       </c>
       <c r="B74" s="1">
-        <v>-22.025279999999999</v>
+        <v>-31.363052419899301</v>
       </c>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
-      <c r="G74" s="1"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A75">
+        <v>0.18980253033321901</v>
+      </c>
+      <c r="B75">
+        <v>-31.2422125628195</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A76">
+        <v>0.20052971764591501</v>
+      </c>
+      <c r="B76">
+        <v>-31.2202416797141</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A77">
+        <v>0.21125690495860999</v>
+      </c>
+      <c r="B77">
+        <v>-31.099401822634299</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A78">
+        <v>0.221984092271306</v>
+      </c>
+      <c r="B78">
+        <v>-31.077430939528899</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A79">
+        <v>0.23271127958400101</v>
+      </c>
+      <c r="B79">
+        <v>-30.956591082449101</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A80">
+        <v>0.24343846689669599</v>
+      </c>
+      <c r="B80">
+        <v>-30.8577221084748</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A81">
+        <v>0.25416565420939202</v>
+      </c>
+      <c r="B81">
+        <v>-30.7918094591586</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A82">
+        <v>0.26489284152208697</v>
+      </c>
+      <c r="B82">
+        <v>-30.7039259267369</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A83">
+        <v>0.27562002883478298</v>
+      </c>
+      <c r="B83">
+        <v>-30.583086069657099</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A84">
+        <v>0.28634721614747799</v>
+      </c>
+      <c r="B84">
+        <v>-30.401826284037501</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A85">
+        <v>0.297074403460173</v>
+      </c>
+      <c r="B85">
+        <v>-30.2754937061814</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A86">
+        <v>0.307801590772869</v>
+      </c>
+      <c r="B86">
+        <v>-30.077755758232598</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A87">
+        <v>0.31852877808556401</v>
+      </c>
+      <c r="B87">
+        <v>-29.9349450180475</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A88">
+        <v>0.32925596539826002</v>
+      </c>
+      <c r="B88">
+        <v>-29.726221628546099</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A89">
+        <v>0.33998315271095503</v>
+      </c>
+      <c r="B89">
+        <v>-29.506512797491901</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A90">
+        <v>0.35071034002364998</v>
+      </c>
+      <c r="B90">
+        <v>-29.2977894079905</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A91">
+        <v>0.36143752733634599</v>
+      </c>
+      <c r="B91">
+        <v>-29.012167927620101</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A92">
+        <v>0.372164714649041</v>
+      </c>
+      <c r="B92">
+        <v>-28.6771119602626</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A93">
+        <v>0.382891901961737</v>
+      </c>
+      <c r="B93">
+        <v>-28.287128785141501</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A94">
+        <v>0.39361908927443201</v>
+      </c>
+      <c r="B94">
+        <v>-27.8257402399278</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A95">
+        <v>0.40434627658712702</v>
+      </c>
+      <c r="B95">
+        <v>-27.303931766174301</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A96">
+        <v>0.41507346389982303</v>
+      </c>
+      <c r="B96">
+        <v>-26.688747039222701</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A97">
+        <v>0.42580065121251798</v>
+      </c>
+      <c r="B97">
+        <v>-25.941737013638701</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A98">
+        <v>0.43652783852521398</v>
+      </c>
+      <c r="B98">
+        <v>-25.024452643987701</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A99">
+        <v>0.44725502583790899</v>
+      </c>
+      <c r="B99">
+        <v>-23.969850254927898</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A100">
+        <v>0.45700701430399598</v>
+      </c>
+      <c r="B100">
+        <v>-22.741311707950199</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A101">
+        <v>0.46578380392347402</v>
+      </c>
+      <c r="B101">
+        <v>-21.438926581646001</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A102">
+        <v>0.47358539469634298</v>
+      </c>
+      <c r="B102">
+        <v>-20.111606246738098</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A103">
+        <v>0.47992418719930002</v>
+      </c>
+      <c r="B103">
+        <v>-18.723386460047902</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A104">
+        <v>0.48577538027895201</v>
+      </c>
+      <c r="B104">
+        <v>-17.434427984530299</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A105">
+        <v>0.492114172781908</v>
+      </c>
+      <c r="B105">
+        <v>-16.046208197840102</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A106">
+        <v>0.49699016701495102</v>
+      </c>
+      <c r="B106">
+        <v>-14.677265245493601</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A107">
+        <v>0.50175780582059404</v>
+      </c>
+      <c r="B107">
+        <v>-13.1815363478617</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A108">
+        <v>0.50587531206183001</v>
+      </c>
+      <c r="B108">
+        <v>-11.7448847136911</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A109">
+        <v>0.51015535144416801</v>
+      </c>
+      <c r="B109">
+        <v>-10.3602613513187</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A110">
+        <v>0.51398648977013095</v>
+      </c>
+      <c r="B110">
+        <v>-8.8993937934080094</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A111">
+        <v>0.51705140043090103</v>
+      </c>
+      <c r="B111">
+        <v>-7.4061584166365497</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A112">
+        <v>0.52081288169639195</v>
+      </c>
+      <c r="B112">
+        <v>-5.9129230398650998</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A113">
+        <v>0.52380813529669001</v>
+      </c>
+      <c r="B113">
+        <v>-4.5146332650849104</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A114">
+        <v>0.52680338889698797</v>
+      </c>
+      <c r="B114">
+        <v>-3.12497490866755</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A115">
+        <v>0.53101377121885396</v>
+      </c>
+      <c r="B115">
+        <v>-1.4734968619106801</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A116">
+        <v>0.53465722246521097</v>
+      </c>
+      <c r="B116">
+        <v>0.507773294793054</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A117">
+        <v>0.53762345229031305</v>
+      </c>
+      <c r="B117">
+        <v>2.0778522711558902</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A118">
+        <v>0.54054904883013899</v>
+      </c>
+      <c r="B118">
+        <v>3.77632359566599</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A119">
+        <v>0.54347464536996504</v>
+      </c>
+      <c r="B119">
+        <v>5.4815082455694197</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A120">
+        <v>0.54611580891286304</v>
+      </c>
+      <c r="B120">
+        <v>7.1464129431129297</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A121">
+        <v>0.54932583844961702</v>
+      </c>
+      <c r="B121">
+        <v>8.9254441723428695</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A122">
+        <v>0.55176383556613895</v>
+      </c>
+      <c r="B122">
+        <v>10.597541718522001</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A123">
+        <v>0.55371423325935598</v>
+      </c>
+      <c r="B123">
+        <v>12.100847083383499</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A124">
+        <v>0.556059354295248</v>
+      </c>
+      <c r="B124">
+        <v>13.7339114376329</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A125">
+        <v>0.55745249550468901</v>
+      </c>
+      <c r="B125">
+        <v>15.194347424625599</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A126">
+        <v>0.55996014968168295</v>
+      </c>
+      <c r="B126">
+        <v>16.705708779959</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A127">
+        <v>0.56135329089112396</v>
+      </c>
+      <c r="B127">
+        <v>18.167007908787902</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A128">
+        <v>0.56346622172544303</v>
+      </c>
+      <c r="B128">
+        <v>19.572778246149301</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A129">
+        <v>0.56581134276133505</v>
+      </c>
+      <c r="B129">
+        <v>21.1828254847645</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A130">
+        <v>0.56769208339407995</v>
+      </c>
+      <c r="B130">
+        <v>22.701187879436699</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A131">
+        <v>0.56976438094312398</v>
+      </c>
+      <c r="B131">
+        <v>24.184832791360499</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A132">
+        <v>0.57221979232476305</v>
+      </c>
+      <c r="B132">
+        <v>25.859327953751599</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A133">
+        <v>0.57461599520500195</v>
+      </c>
+      <c r="B133">
+        <v>27.7157734152314</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A134">
+        <v>0.57695647243686299</v>
+      </c>
+      <c r="B134">
+        <v>29.335631699385701</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A135">
+        <v>0.57939446955338403</v>
+      </c>
+      <c r="B135">
+        <v>31.2103278154705</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A136">
+        <v>0.58036966839999304</v>
+      </c>
+      <c r="B136">
+        <v>35.996928820908103</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A137">
+        <v>0.58085726782329705</v>
+      </c>
+      <c r="B137">
+        <v>32.311313179975102</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A138">
+        <v>0.58232006609320996</v>
+      </c>
+      <c r="B138">
+        <v>37.447007105865303</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A139">
+        <v>0.584270463786428</v>
+      </c>
+      <c r="B139">
+        <v>39.138765104982099</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A140">
+        <v>0.58638339462074596</v>
+      </c>
+      <c r="B140">
+        <v>40.715725239873102</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A141">
+        <v>0.58865885859616696</v>
+      </c>
+      <c r="B141">
+        <v>42.476966156810697</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A142">
+        <v>0.59099933582802699</v>
+      </c>
+      <c r="B142">
+        <v>44.546348709301803</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A143">
+        <v>0.59304725340590603</v>
+      </c>
+      <c r="B143">
+        <v>46.318666613138497</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A144">
+        <v>0.59534593640148303</v>
+      </c>
+      <c r="B144">
+        <v>48.378698462403101</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A145">
+        <v>0.59743564821564499</v>
+      </c>
+      <c r="B145">
+        <v>50.354214340198297</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A146">
+        <v>0.59997116521682703</v>
+      </c>
+      <c r="B146">
+        <v>52.522642418402903</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A147">
+        <v>0.60176986531168297</v>
+      </c>
+      <c r="B147">
+        <v>54.596196823102702</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A148">
+        <v>0.60353064100694898</v>
+      </c>
+      <c r="B148">
+        <v>56.6571877188521</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A149">
+        <v>0.60572483841181801</v>
+      </c>
+      <c r="B149">
+        <v>58.642318037656999</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A150">
+        <v>0.60762105839133496</v>
+      </c>
+      <c r="B150">
+        <v>60.832876113497498</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A151">
+        <v>0.60946310065715203</v>
+      </c>
+      <c r="B151">
+        <v>62.8710417029097</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A152">
+        <v>0.61157603149147</v>
+      </c>
+      <c r="B152">
+        <v>65.107250391424699</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A153">
+        <v>0.61373540036610397</v>
+      </c>
+      <c r="B153">
+        <v>67.177927656670207</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A154">
+        <v>0.61450162803129604</v>
+      </c>
+      <c r="B154">
+        <v>68.744530089525796</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A155">
+        <v>0.61547682687790495</v>
+      </c>
+      <c r="B155">
+        <v>70.194608374483096</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A156">
+        <v>0.61645202572451396</v>
+      </c>
+      <c r="B156">
+        <v>71.535355360177704</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A157">
+        <v>0.61856495655883303</v>
+      </c>
+      <c r="B157">
+        <v>73.474067829120202</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A158">
+        <v>0.61937762226434001</v>
+      </c>
+      <c r="B158">
+        <v>75.320232312283295</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A159">
+        <v>0.62153699113897298</v>
+      </c>
+      <c r="B159">
+        <v>76.827853386326197</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A160">
+        <v>0.62230321880416595</v>
+      </c>
+      <c r="B160">
+        <v>78.321088763097606</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A161">
+        <v>0.62327841765077396</v>
+      </c>
+      <c r="B161">
+        <v>79.618998339139594</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>